<commit_message>
Change Credit Card data type to 'text'
This is because when you enter a number over 12 digits in an Excel spreadsheet, it auto-corrects the number to scientific notation.

Which is something we don't want when displaying Credit Card Numbers.
</commit_message>
<xml_diff>
--- a/personal_information.xlsx
+++ b/personal_information.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhati\Documents\GitHub\Anonymize_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9A4AFC-8410-4B94-B178-B2D50E3A119A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFAE7CB-7309-47E5-A03D-1B80E3B17974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F532BE12-EBAC-48E5-A755-B1EA3172AA76}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>Credit Card Number</t>
+  </si>
+  <si>
+    <t>378282246310005</t>
+  </si>
+  <si>
+    <t>5610591081018250</t>
   </si>
 </sst>
 </file>
@@ -119,10 +125,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -461,7 +468,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -509,8 +516,8 @@
       <c r="E2" s="2">
         <v>38580.860659722224</v>
       </c>
-      <c r="F2">
-        <v>378282246310005</v>
+      <c r="F2" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -529,8 +536,8 @@
       <c r="E3" s="2">
         <v>38584.312743055554</v>
       </c>
-      <c r="F3">
-        <v>5610591081018250</v>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -540,5 +547,8 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+  <ignoredErrors>
+    <ignoredError sqref="F2:F3" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>